<commit_message>
copied quiz sheets from gradingapp, changed titles for m13
</commit_message>
<xml_diff>
--- a/quizsheets/dsaide_stochasticsir.xlsx
+++ b/quizsheets/dsaide_stochasticsir.xlsx
@@ -466,7 +466,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Report the integer</t>
+          <t>Report the rounded integer</t>
         </is>
       </c>
     </row>
@@ -493,7 +493,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Report the integer</t>
+          <t>Report the rounded integer</t>
         </is>
       </c>
     </row>
@@ -520,7 +520,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Report the integer</t>
+          <t>Report to one decimal place</t>
         </is>
       </c>
     </row>

</xml_diff>